<commit_message>
edit docker-compose.yml (add volume data)
</commit_message>
<xml_diff>
--- a/data/air_bd.xlsx
+++ b/data/air_bd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frexr\PycharmProjects\AirportDirectory\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Мой диск\Проекты\AirportDirectory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2883AD05-FEA4-4C69-9FC9-E7F41815E1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13494971-4534-4101-BC4C-8239FE2A1C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="9432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="130">
   <si>
     <t>name</t>
   </si>
@@ -64,24 +64,413 @@
     <t>img_airport</t>
   </si>
   <si>
+    <t>Шереметьево</t>
+  </si>
+  <si>
+    <t>Международный аэропорт Шереметьево им. А. С. Пушкина</t>
+  </si>
+  <si>
+    <t>Москва</t>
+  </si>
+  <si>
+    <t>Московская обл., Химки, Международное шоссе, 1</t>
+  </si>
+  <si>
+    <t>https://www.svo.aero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шереметьево — крупнейший российский аэропорт, расположенный в 28 км от центра Москвы и в 11 км от МКАД. Каждый год услугами аэропорта пользуется свыше 14 млн авиапутешественников. </t>
+  </si>
+  <si>
+    <t>Шереметьево — крупнейший российский аэропорт, расположенный в 28 км от центра Москвы и в 11 км от МКАД. Каждый год услугами аэропорта пользуется свыше 14 млн авиапутешественников. Аэропорт имеет III А категорию ICAO, которая позволяет осуществлять полеты самолетов без ограничения по высоте и при ограниченной видимости на ВПП (не менее 200 м).
+Аэропорт имеет два сектора: Шереметьево-1 (Ш-1), обслуживающий перевозки на внутренних авиалиниях и стран СНГ, Шереметьево-2 (Ш-2), где осуществляются только международные полеты.
+12 марта 2007г. был открыт новый современный терминал С. Терминал располагается рядом с Шереметьево-1 и обслуживает регулярные и чартерные международные рейсы.
+В 2009 году первых пассажиров принял Шереметьево-3, которое соединено крыльями с Шереметьево-2 и железнодорожной станцией.</t>
+  </si>
+  <si>
+    <t>UUEE</t>
+  </si>
+  <si>
+    <t>SVO</t>
+  </si>
+  <si>
+    <t>ШРМ</t>
+  </si>
+  <si>
+    <t>55.966324</t>
+  </si>
+  <si>
+    <t>37.416573</t>
+  </si>
+  <si>
+    <t>Домодедово</t>
+  </si>
+  <si>
+    <t>Международный аэропорт Домодедово имени М. В. Ломоносова</t>
+  </si>
+  <si>
+    <t>Московская обл., Домодедово, Аэропорт, 1</t>
+  </si>
+  <si>
+    <t>https://dme.ru</t>
+  </si>
+  <si>
+    <t>Домодедово — крупнейший аэропорт Российской Федерации, расположен в г. Домодедово, Московской области. Обслуживает как внутрироссийские так и международные авиарейсы.</t>
+  </si>
+  <si>
+    <t>Домодедово — крупнейший аэропорт Российской Федерации, расположен в г. Домодедово, Московской области. Обслуживает как внутрироссийские так и международные авиарейсы. Аэропорт управляется компанией ИстЛайн. Внутренний и международный терминалы расположены в одном здании.
+Аэропортовый комплекс включает в себя лётное поле, образованное двумя независимыми параллельными взлётно-посадочными полосами (ВПП-1 и ВПП-2). Они расположены в двух километрах друг от друга, что делает Домодедово единственным аэропортом Московского авиационного узла, способным одновременно производить на своих полосах операции по взлёту и посадке. Обе ВПП сертифицированы по категории ICAO CAT IIIА. Реконструкция ВПП-1 сделала Домодедово первым российским аэропортом, имеющим возможности принимать пассажирский лайнер Airbus A380.
+Доля пассажиропотока аэропорта от общего объёма в Москве составляет 32,3 %. Рейсы из аэропорта Домодедово выполняют 30 авиакомпаний по более чем 80 направлениям для путешествий: 49 из них — по России, 22 — по странам ближнего зарубежья и 13 — по странам дальнего зарубежья. Среди уникальных для Московского авиационного узла направлений, по которым можно отправиться в путешествие только из аэропорта Домодедово: Благовещенск, Братск, Бугульма, Курган, Кызыл, Норильск, Сабетта, Тобольск, Чита, Куляб, Ленкорань, Навои, Нукус, Тамчы, Кутаиси, Аддис-Абеба, Бахрейн, Касабланка, Кувейт, Шарджа и Тель-Авив.</t>
+  </si>
+  <si>
+    <t>UUDD</t>
+  </si>
+  <si>
+    <t>DME</t>
+  </si>
+  <si>
+    <t>ДМД</t>
+  </si>
+  <si>
+    <t>55.414566</t>
+  </si>
+  <si>
+    <t>37.899494</t>
+  </si>
+  <si>
+    <t>Пулково</t>
+  </si>
+  <si>
+    <t>Международный аэропорт Пулково</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург</t>
+  </si>
+  <si>
+    <t>г. Санкт-Петербург, Пулковское ш., д. 41, лит. ЗА</t>
+  </si>
+  <si>
+    <t>http://www.pulkovoairport.ru</t>
+  </si>
+  <si>
+    <t>Крупнейший аэропорт Северо-Запада России, важный транспортный узел.</t>
+  </si>
+  <si>
+    <t>Пулково — крупнейший аэропорт России. В 2008 году занял четвертое место по количеству перевезенных пассажиров среди всех аэропортов России. Пассажиропоток аэропорта за 2008 год превысил 7 млн человек. Аэропорт имеет сертификат ИСО 9001:2000 и множество наград на международных и всероссийских конкурсах.
+День рождения авиапредприятие отмечает 24 июня. Именно в этот день в 1932 году был сдан в эксплуатацию аэродром «Шоссейная», получивший наименование по названию ближайшей железнодорожной станции. А 25 апреля 1973 года аэропорт получил новое и современное имя — «Пулково».
+Второй аэровокзальный комплекс «Пулково-2» был открыт в 1980 году. 
+11 апреля 1986 года аэровокзал «Пулково-2» был обновлён: справа и слева от старого здания пристроили два павильона. Ввод аэровокзального комплекса позволил обслуживать в два раза больше пассажиров международных рейсов.</t>
+  </si>
+  <si>
+    <t>ULLI</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>ПЛК</t>
+  </si>
+  <si>
+    <t>59.806084</t>
+  </si>
+  <si>
+    <t>30.3083</t>
+  </si>
+  <si>
+    <t>Сочи (Адлер)</t>
+  </si>
+  <si>
+    <t>Международный аэропорт Сочи имени В. И. Севастьянова</t>
+  </si>
+  <si>
+    <t>Адлер</t>
+  </si>
+  <si>
+    <t>Краснодарский край, Адлерский р-н, ул. Мира, 50</t>
+  </si>
+  <si>
+    <t>https://aer.aero</t>
+  </si>
+  <si>
+    <t>Международный аэропорт Со́чи  — международный аэропорт города Сочи, Краснодарский край. Крупнейший узел местных и международных авиалиний в Южном федеральном округе России.</t>
+  </si>
+  <si>
+    <t>Международный аэропорт Со́чи  — международный аэропорт города Сочи, Краснодарский край. Крупнейший узел местных и международных авиалиний в Южном федеральном округе России.
+Расположен в Адлерском районе Сочи, из-за чего также распространено название «аэропорт Адлер». Обслуживает крупнейший российский курорт, его агломерацию (включая федеральную территорию Сириус, Туапсе). Имеет статус аэропорта федерального значения.
+Аэропорт занимает в стране 5-е место по пассажирообороту (11 076 621 пассажиров) после московских Шереметьево, Домодедово, Внуково и петербургского Пулково.
+Аэродром первого класса, имеет две искусственные взлётно-посадочные полосы, сеть рулёжных дорожек общей протяжённостью 4310 м при ширине 40,5 м, перрон и места стоянок общей площадью 219 тыс. м². Особенностью аэродрома является то, что из-за наличия естественных препятствий (гор) к северу и северо-востоку от аэродрома, посадка производится только с одной стороны — со стороны моря. По этой же причине взлёт производится в строго обратном направлении.
+Аэропорт Сочи сертифицирован Авиационным регистром МАК на пригодность к международным полётам. С 2007 года годен к эксплуатации всех типов воздушных судов, в том числе: А-330 и его модификации, Боинг-747, Боинг-777 (-200, −300, −200LR, −300ER).
+Новое здание аэровокзала построено в 1989—2007 годах, площадью 65 000 м² и является одним из крупнейших в России. В конце 2013 года завершены строительство новой посадочной галереи и 10 телетрапов . Существует возможность парковки более 1000 автомобилей. Пропускная способность аэровокзального комплекса — 2 500 пасс./час. В декабре 2013 года в эксплуатацию был введён новый VIP-терминал. Площадь терминала 4 тысячи квадратных метров. Он построен рядом с основным аэропортовым комплексом. В терминале — пять помещений для деловых мероприятий и встреч.</t>
+  </si>
+  <si>
+    <t>URSS</t>
+  </si>
+  <si>
+    <t>AER</t>
+  </si>
+  <si>
+    <t>АДЛ</t>
+  </si>
+  <si>
+    <t>43.44884</t>
+  </si>
+  <si>
+    <t>39.941105</t>
+  </si>
+  <si>
+    <t>Кольцово (Екатеринбург)</t>
+  </si>
+  <si>
+    <t>Аэропорт «Кольцово» имени А. Н. Демидова</t>
+  </si>
+  <si>
+    <t>Екатеринбург</t>
+  </si>
+  <si>
+    <t>Свердловская обл., г. Екатеринбург, ул. Бахчиванджи, 1</t>
+  </si>
+  <si>
+    <t>https://svx.aero</t>
+  </si>
+  <si>
+    <t>Крупнейший аэропорт Урала, важный транспортный узел между Европой и Азией</t>
+  </si>
+  <si>
+    <t>Аэропорт «Кольцово» имени А. Н. Демидова — международный аэропорт Екатеринбурга с аэродромом класса «Б», расположенный в микрорайоне Кольцово Октябрьского района, что в 16 километрах к юго-востоку от центра города и в девяти километрах к северу от города Арамиль. Обслуживает как сам Екатеринбург, так прилежащие к нему районы Свердловской области. Имеет статус аэропорта федерального значения.
+На протяжении 10 лет (до 2015 года) являлся пятым по объёму годового пассажиропотока аэропортом России, в настоящее время занимает седьмое место по этому показателю. Так, за 2020 год аэропорт Кольцово обслужил около 3,5 млн человек. Грузопоток аэропорта за 2016 год превысил 27,6 тысяч тонн груза и почты.
+В аэропорту расположена главная техническая база и штаб-квартира российской авиакомпании «Уральские авиалинии», для которой Кольцово является и главным хабом.
+Аэродром Кольцово первого класса имеет две ВПП, 72 стоянки для самолётов, а также допуск на приём всех (кроме Airbus A380) современных типов воздушных судов российского и зарубежного производства, включая Ил-96, Airbus A330, Airbus A340, Airbus A350, Boeing 777, Boeing 787.
+В 2006 открыт новый международный терминал. В октябре 2007 введён в строй новый терминал внутренних авиалиний. На месте старого терминала в 2009 году возведён новый внутренний терминал, а прежний объединён с международным терминалом. В результате, аэропорт стал одним из самых современных в России. После ввода в эксплуатацию нового терминала пропускная способность аэропорта приблизилась к 8 миллионам 400 тысячам пассажиров в год. В составе аэропорта современная гостиница, терминал деловой авиации.</t>
+  </si>
+  <si>
+    <t>USSS</t>
+  </si>
+  <si>
+    <t>SVX</t>
+  </si>
+  <si>
+    <t>КЛЦ</t>
+  </si>
+  <si>
+    <t>56.750336</t>
+  </si>
+  <si>
+    <t>60.804314</t>
+  </si>
+  <si>
+    <t>Толмачёво (Новосибирск)</t>
+  </si>
+  <si>
+    <t>Международный аэропо́рт Новосибирск (Толмачёво) имени А. И. Покрышкина</t>
+  </si>
+  <si>
+    <t>Новосибирск</t>
+  </si>
+  <si>
+    <t>Новосибирская область, город Обь-4, аэропорт Толмачево.</t>
+  </si>
+  <si>
+    <t>http://tolmachevo.ru</t>
+  </si>
+  <si>
+    <t>Аэропорт Толмачёво находится в России и обслуживает г. Новосибирск. Толмачёво расположен в 17 км от центра города. В аэропорту Толмачёво (Tolmachevo) работают 2 терминала. В этот аэропорт прилетают как регулярные рейсы 32 авиакомпаний, так и чартеры. Город Новосибирск не располагает другими аэропортами.</t>
+  </si>
+  <si>
+    <t>Междунаро́дный аэропо́рт Новосиби́рск (Толмачёво) имени А. И. Покры́шкина — международный аэропорт, обслуживающий Новосибирск, расположен в городе Обь Новосибирской области, в 17 км от Новосибирска. Крупнейший за Уралом по пассажиропотоку. Аэропорт находится на пересечении большого числа воздушных линий, идущих из Юго-Восточной Азии в Европу и из Северной Америки в Индию и Азию. Регулярными пассажирскими рейсами аэропорт связан со многими крупнейшими городами России и стран СНГ, а также с ОАЭ, Турцией, Тунисом, Танзанией, Болгарией, Германией, Испанией, Италией, Индией, Индонезией, Японией, Китаем, Южной Кореей, Чехией, Грецией, Кипром, Вьетнамом и Таиландом.
+Аэропорт Толмачёво имеет платиновый сертификат IATA, подтверждающий 100%-е внедрение инновационной технологии по упрощению аэропортовых формальностей BCBP, Толмачёво — четвёртый аэропорт в России после Домодедово, Шереметьево и Пулково, полностью внедривший технологию BCBP (кодирование посадочных талонов с использованием двумерных штрихкодов — Bar coded boarding passes).
+Был открыт в 1957 году, а в 1992 году аэропорту был присвоен статус международного. В 2004 году одержал победу в конкурсе "Лучший аэропорт России и СНГ". Сегодня аэропорт относится к классу А и может принимать все виды воздушных судов.
+Аэропорт является узловым для S7 Airlines.</t>
+  </si>
+  <si>
+    <t>UNNT</t>
+  </si>
+  <si>
+    <t>OVB</t>
+  </si>
+  <si>
+    <t>ТЛЧ</t>
+  </si>
+  <si>
+    <t>55.00901</t>
+  </si>
+  <si>
+    <t>82.667</t>
+  </si>
+  <si>
+    <t>Ростов-на-Дону (Платов)</t>
+  </si>
+  <si>
+    <t>Международный аэропорт Ростова-на-Дону «Платов»</t>
+  </si>
+  <si>
+    <t>Ростов-на-Дону</t>
+  </si>
+  <si>
+    <t>Ростовская область, Аксайский район, аэропорт Платов</t>
+  </si>
+  <si>
+    <t>https://rov.aero</t>
+  </si>
+  <si>
+    <t>Аэропорт Пла́тов  — международный аэропорт Ростова-на-Дону, преемник старого аэропорта на проспекте Шолохова. Расположен в 29 километрах к северо-востоку от Ростова-на-Дону в Аксайском районе Ростовской области, в 15 км к северо-западу от города Новочеркасска (в 4 км к северу от станицы Грушевской, вблизи федеральной автотрассы М-4). Назван в честь казачьего атамана Матвея Платова.</t>
+  </si>
+  <si>
+    <t>Аэропорт Пла́тов  — международный аэропорт Ростова-на-Дону, преемник старого аэропорта на проспекте Шолохова. Расположен в 29 километрах к северо-востоку от Ростова-на-Дону в Аксайском районе Ростовской области, в 15 км к северо-западу от города Новочеркасска (в 4 км к северу от станицы Грушевской, вблизи федеральной автотрассы М-4). Назван в честь казачьего атамана Матвея Платова.
+Новый аэропорт Ростова построен в рамках подготовки к чемпионату мира по футболу 2018 года. Первый в современной истории России построенный с нуля крупный аэропорт, третий по пассажирообороту (после Сочи и Краснодара) в Южном федеральном округе. Для регулярных рейсов аэропорт открыт с 7 декабря 2017 года.
+Аэродром допущен к приёму самолётов Airbus A310, Airbus A319, Airbus A320, Airbus A321, Airbus A330, Boeing 737, Boeing 747, Boeing 757, Boeing 767, Вoeing-777, CRJ, Ан-124, Ил-62, Ил-76, Ту-154, Ту-204 и всех более лёгких, а также вертолётов всех типов. Классификационное число ВПП (PCN) 57/R/A/W/T, ИВПП оборудована по II категории ИКАО.
+В феврале 2019 года аэропорт получил рейтинг 5 звёзд по итогам аудита, проведённого экспертами авторитетной международной рейтинговой организации Skytrax (Великобритания). Такой оценки российский аэропорт удостоен впервые за все время существования рейтинга с 1989 года. В 2019 году аэропорт показал наибольший отток пассажиропотока среди 30 крупнейших аэропортов России, эксперты называют причиной данного падения высокие тарифы аэропорта на обслуживание авиакомпаний.</t>
+  </si>
+  <si>
+    <t>URRP</t>
+  </si>
+  <si>
+    <t>ROV</t>
+  </si>
+  <si>
+    <t>РОВ</t>
+  </si>
+  <si>
+    <t>47.49417</t>
+  </si>
+  <si>
+    <t>39.92472</t>
+  </si>
+  <si>
     <t>https://www.aviasales.ru/airports/sheremetevo</t>
   </si>
   <si>
+    <t>sheremetevo.jpg</t>
+  </si>
+  <si>
+    <t>domodedovo.jpg</t>
+  </si>
+  <si>
+    <t>sochi.jpg</t>
+  </si>
+  <si>
+    <t>kolcovo.jpg</t>
+  </si>
+  <si>
+    <t>tolmacheva.jpg</t>
+  </si>
+  <si>
+    <t>platov.jpg</t>
+  </si>
+  <si>
+    <t>sheremetevo.webp</t>
+  </si>
+  <si>
+    <t>Внуково</t>
+  </si>
+  <si>
+    <t>VKO</t>
+  </si>
+  <si>
+    <t>UUWW</t>
+  </si>
+  <si>
+    <t>https://www.vnukovo.ru/</t>
+  </si>
+  <si>
+    <t>ВНК</t>
+  </si>
+  <si>
+    <r>
+      <t>Международный аэропорт Внуково имени </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>А. Н. Туполева</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Международный аэропорт Внуково — старейшее из ныне действующих авиапредприятий московского авиационного узла и один из крупнейших авиатранспортных комплексов России. Маршрутная сеть аэропорта охватывает всю территорию России, а также страны ближнего и дальнего зарубежья. Международный аэропорт Внуково в 2019 году побил исторический рекорд и обслужил свыше 24 млн пассажиров.
+Международный аэропорт Внуково — самый близкий к центру столицы и единственный аэропорт, расположенный на территории Москвы.
+Аэродромный комплекс Внуково располагает двумя современными взлетно-посадочными полосами, длиной 3 500 и 3 060 м, аэродромная пропускная способность составляет 58 взлетно-посадочных операций в час. Аэровокзальный комплекс Внуково общей площадью около 300 тыс. кв. м способен обеспечить пропускную способность до 35 млн пассажиров в год.
+Аэропорт состоит из трёх пассажирских терминалов и грузового терминала «Внуково-Карго». Основной пассажирский комплекс «Внуково-1» состоит из терминалов «A», «B» и «D». Комплекс «Внуково-2» используется для обслуживания спецрейсов высших руководителей России (в том числе президента и председателя Правительства), а также руководителей других стран. Терминалы «Внуково-3» обслуживают рейсы бизнес-авиации, спецрейсов правительства Москвы и авиации Роскосмоса.
+Аэропорту присвоен третий (наивысший) уровень координации по классификации IATA.
+23 марта 2012 года в аэропорту состоялся презентационный прилёт крупнейшего в мире пассажирского авиалайнера Airbus А380 авиакомпании Lufthansa, а 9 апреля — пассажирского самолёта Boeing 787 Dreamliner.
+</t>
+  </si>
+  <si>
+    <t>Международный аэропорт Внуково — самый близкий к центру столицы и единственный аэропорт, расположенный на территории Москвы. Один из крупнейших авиатранспортных комплексов России.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Московская область, посёлок Внуково, улица 2-я Рейсовая, 2</t>
+  </si>
+  <si>
+    <t>55.5996</t>
+  </si>
+  <si>
+    <t>37.2712</t>
+  </si>
+  <si>
+    <t>vnukovo.jpg</t>
+  </si>
+  <si>
+    <t>vnukovo.webp</t>
+  </si>
+  <si>
+    <t>Europe/Moscow</t>
+  </si>
+  <si>
+    <t>Asia/Yekaterinburg</t>
+  </si>
+  <si>
+    <t>Asia/Novosibirsk</t>
+  </si>
+  <si>
     <t>time_zone</t>
   </si>
   <si>
+    <t>https://www.svo.aero/ru/departure/timetable</t>
+  </si>
+  <si>
     <t>online_tablo</t>
+  </si>
+  <si>
+    <t>https://www.vnukovo.ru/ru/for-passengers/reysi/online-tablo</t>
+  </si>
+  <si>
+    <t>https://www.dme.ru/flight/live-board/</t>
+  </si>
+  <si>
+    <t>https://ar-rov.ru/board/</t>
+  </si>
+  <si>
+    <t>https://aer.aero/flights/online-schedule/</t>
+  </si>
+  <si>
+    <t>https://ar-svx.ru/board/</t>
+  </si>
+  <si>
+    <t>https://tolmachevo.ru/passengers/information/timetable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -166,31 +555,31 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -423,28 +812,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.453125" bestFit="1"/>
-    <col min="2" max="2" width="21.453125"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="45.90625" bestFit="1"/>
-    <col min="5" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="19.08984375" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" bestFit="1"/>
-    <col min="12" max="12" width="10.36328125" customWidth="1"/>
-    <col min="13" max="13" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1"/>
+    <col min="2" max="2" width="21.44140625"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="45.88671875" bestFit="1"/>
+    <col min="5" max="6" width="25.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" bestFit="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,159 +877,430 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="8"/>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P3" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="2"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P4" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="2"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P5" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="2"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P6" t="s">
+        <v>127</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="2"/>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="P7" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="2"/>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P8" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="2"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P9" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A26" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A26" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="P2" r:id="rId9" xr:uid="{540F9E2E-CA77-4988-B1B1-557E6D1E6A06}"/>
   </hyperlinks>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit data airport v1
</commit_message>
<xml_diff>
--- a/data/air_bd.xlsx
+++ b/data/air_bd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Мой диск\Проекты\AirportDirectory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frexr\PycharmProjects\AirportDirectory\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13494971-4534-4101-BC4C-8239FE2A1C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065B4D9A-EE3E-4F8A-9E25-C69A7D9F9C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="9432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="132">
   <si>
     <t>name</t>
   </si>
@@ -452,6 +452,12 @@
   </si>
   <si>
     <t>https://tolmachevo.ru/passengers/information/timetable</t>
+  </si>
+  <si>
+    <t>platov.webp</t>
+  </si>
+  <si>
+    <t>pulkovo.jpg</t>
   </si>
 </sst>
 </file>
@@ -579,7 +585,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -812,28 +818,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1"/>
-    <col min="2" max="2" width="21.44140625"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="45.88671875" bestFit="1"/>
-    <col min="5" max="6" width="25.44140625" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" bestFit="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" bestFit="1"/>
+    <col min="2" max="2" width="21.453125"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="45.90625" bestFit="1"/>
+    <col min="5" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="19.08984375" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" bestFit="1"/>
+    <col min="12" max="12" width="10.36328125" customWidth="1"/>
+    <col min="13" max="13" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -883,7 +889,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -933,7 +939,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>105</v>
       </c>
@@ -983,7 +989,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -1033,7 +1039,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -1071,10 +1077,10 @@
         <v>48</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>118</v>
@@ -1083,7 +1089,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1133,7 +1139,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
@@ -1183,7 +1189,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
@@ -1233,7 +1239,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
@@ -1271,7 +1277,7 @@
         <v>96</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>103</v>
@@ -1283,7 +1289,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>97</v>
       </c>

</xml_diff>